<commit_message>
#219 channel codes changed
</commit_message>
<xml_diff>
--- a/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2019-11-29/5_families.xlsx
+++ b/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2019-11-29/5_families.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -37,13 +37,10 @@
     <t xml:space="preserve">attribute_as_label</t>
   </si>
   <si>
-    <t xml:space="preserve">requirements-print</t>
-  </si>
-  <si>
-    <t xml:space="preserve">requirements-ecommerce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">requirements-mobile</t>
+    <t xml:space="preserve">requirements-GS1_GDSN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requirements-PRODUCT_CATALOG</t>
   </si>
   <si>
     <t xml:space="preserve">MD_RECIPIENT_MAPPING</t>
@@ -235,22 +232,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1592592592593"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.44814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3111111111111"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="59"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.2962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="59.1407407407407"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.44814814814815"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -272,169 +269,145 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>